<commit_message>
Update json file & rerun GSW notebooks
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X129"/>
+  <dimension ref="A1:Y135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +549,11 @@
           <t>+/-</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>PO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -631,6 +636,7 @@
       <c r="X2" t="n">
         <v>36</v>
       </c>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -713,6 +719,7 @@
       <c r="X3" t="n">
         <v>-36</v>
       </c>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -795,6 +802,7 @@
       <c r="X4" t="n">
         <v>41</v>
       </c>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -877,6 +885,7 @@
       <c r="X5" t="n">
         <v>-41</v>
       </c>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -959,6 +968,7 @@
       <c r="X6" t="n">
         <v>8</v>
       </c>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1041,6 +1051,7 @@
       <c r="X7" t="n">
         <v>-8</v>
       </c>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1123,6 +1134,7 @@
       <c r="X8" t="n">
         <v>-18</v>
       </c>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1205,6 +1217,7 @@
       <c r="X9" t="n">
         <v>18</v>
       </c>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1287,6 +1300,7 @@
       <c r="X10" t="n">
         <v>-15</v>
       </c>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1369,6 +1383,7 @@
       <c r="X11" t="n">
         <v>15</v>
       </c>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1451,6 +1466,7 @@
       <c r="X12" t="n">
         <v>6</v>
       </c>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1533,6 +1549,7 @@
       <c r="X13" t="n">
         <v>-6</v>
       </c>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1615,6 +1632,7 @@
       <c r="X14" t="n">
         <v>13</v>
       </c>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1697,6 +1715,7 @@
       <c r="X15" t="n">
         <v>-13</v>
       </c>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1779,6 +1798,7 @@
       <c r="X16" t="n">
         <v>6</v>
       </c>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1861,6 +1881,7 @@
       <c r="X17" t="n">
         <v>-6</v>
       </c>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1943,6 +1964,7 @@
       <c r="X18" t="n">
         <v>-19</v>
       </c>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2025,6 +2047,7 @@
       <c r="X19" t="n">
         <v>19</v>
       </c>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2107,6 +2130,7 @@
       <c r="X20" t="n">
         <v>11</v>
       </c>
+      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2189,6 +2213,7 @@
       <c r="X21" t="n">
         <v>-11</v>
       </c>
+      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2271,6 +2296,7 @@
       <c r="X22" t="n">
         <v>-3</v>
       </c>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2353,6 +2379,7 @@
       <c r="X23" t="n">
         <v>3</v>
       </c>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2435,6 +2462,7 @@
       <c r="X24" t="n">
         <v>-5</v>
       </c>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2517,6 +2545,7 @@
       <c r="X25" t="n">
         <v>5</v>
       </c>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2599,6 +2628,7 @@
       <c r="X26" t="n">
         <v>-3</v>
       </c>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2681,6 +2711,7 @@
       <c r="X27" t="n">
         <v>3</v>
       </c>
+      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2763,6 +2794,7 @@
       <c r="X28" t="n">
         <v>-23</v>
       </c>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2845,6 +2877,7 @@
       <c r="X29" t="n">
         <v>23</v>
       </c>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2927,6 +2960,7 @@
       <c r="X30" t="n">
         <v>4</v>
       </c>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3009,6 +3043,7 @@
       <c r="X31" t="n">
         <v>-4</v>
       </c>
+      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3091,6 +3126,7 @@
       <c r="X32" t="n">
         <v>-10</v>
       </c>
+      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3173,6 +3209,7 @@
       <c r="X33" t="n">
         <v>10</v>
       </c>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -3255,6 +3292,7 @@
       <c r="X34" t="n">
         <v>8</v>
       </c>
+      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3337,6 +3375,7 @@
       <c r="X35" t="n">
         <v>-8</v>
       </c>
+      <c r="Y35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3419,6 +3458,7 @@
       <c r="X36" t="n">
         <v>4</v>
       </c>
+      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3501,6 +3541,7 @@
       <c r="X37" t="n">
         <v>-4</v>
       </c>
+      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3583,6 +3624,7 @@
       <c r="X38" t="n">
         <v>-8</v>
       </c>
+      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3665,6 +3707,7 @@
       <c r="X39" t="n">
         <v>8</v>
       </c>
+      <c r="Y39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3747,6 +3790,7 @@
       <c r="X40" t="n">
         <v>-4</v>
       </c>
+      <c r="Y40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3829,6 +3873,7 @@
       <c r="X41" t="n">
         <v>4</v>
       </c>
+      <c r="Y41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3911,6 +3956,7 @@
       <c r="X42" t="n">
         <v>-6</v>
       </c>
+      <c r="Y42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3993,6 +4039,7 @@
       <c r="X43" t="n">
         <v>6</v>
       </c>
+      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -4075,6 +4122,7 @@
       <c r="X44" t="n">
         <v>17</v>
       </c>
+      <c r="Y44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -4157,6 +4205,7 @@
       <c r="X45" t="n">
         <v>-17</v>
       </c>
+      <c r="Y45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4239,6 +4288,7 @@
       <c r="X46" t="n">
         <v>-8</v>
       </c>
+      <c r="Y46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -4321,6 +4371,7 @@
       <c r="X47" t="n">
         <v>8</v>
       </c>
+      <c r="Y47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -4403,6 +4454,7 @@
       <c r="X48" t="n">
         <v>-1</v>
       </c>
+      <c r="Y48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4485,6 +4537,7 @@
       <c r="X49" t="n">
         <v>1</v>
       </c>
+      <c r="Y49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4567,6 +4620,7 @@
       <c r="X50" t="n">
         <v>10</v>
       </c>
+      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4649,6 +4703,7 @@
       <c r="X51" t="n">
         <v>-10</v>
       </c>
+      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4731,6 +4786,7 @@
       <c r="X52" t="n">
         <v>-51</v>
       </c>
+      <c r="Y52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -4813,6 +4869,7 @@
       <c r="X53" t="n">
         <v>51</v>
       </c>
+      <c r="Y53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -4895,6 +4952,7 @@
       <c r="X54" t="n">
         <v>10</v>
       </c>
+      <c r="Y54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -4977,6 +5035,7 @@
       <c r="X55" t="n">
         <v>-10</v>
       </c>
+      <c r="Y55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -5059,6 +5118,7 @@
       <c r="X56" t="n">
         <v>6</v>
       </c>
+      <c r="Y56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -5141,6 +5201,7 @@
       <c r="X57" t="n">
         <v>-6</v>
       </c>
+      <c r="Y57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -5223,6 +5284,7 @@
       <c r="X58" t="n">
         <v>2</v>
       </c>
+      <c r="Y58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -5305,6 +5367,7 @@
       <c r="X59" t="n">
         <v>-2</v>
       </c>
+      <c r="Y59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -5387,6 +5450,7 @@
       <c r="X60" t="n">
         <v>-10</v>
       </c>
+      <c r="Y60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -5469,6 +5533,7 @@
       <c r="X61" t="n">
         <v>10</v>
       </c>
+      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -5551,6 +5616,7 @@
       <c r="X62" t="n">
         <v>-4</v>
       </c>
+      <c r="Y62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5633,6 +5699,7 @@
       <c r="X63" t="n">
         <v>4</v>
       </c>
+      <c r="Y63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -5715,6 +5782,7 @@
       <c r="X64" t="n">
         <v>18</v>
       </c>
+      <c r="Y64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -5797,6 +5865,7 @@
       <c r="X65" t="n">
         <v>-18</v>
       </c>
+      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -5879,6 +5948,7 @@
       <c r="X66" t="n">
         <v>-34</v>
       </c>
+      <c r="Y66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -5961,6 +6031,7 @@
       <c r="X67" t="n">
         <v>34</v>
       </c>
+      <c r="Y67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -6043,6 +6114,7 @@
       <c r="X68" t="n">
         <v>-8</v>
       </c>
+      <c r="Y68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -6125,6 +6197,7 @@
       <c r="X69" t="n">
         <v>8</v>
       </c>
+      <c r="Y69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -6207,6 +6280,7 @@
       <c r="X70" t="n">
         <v>30</v>
       </c>
+      <c r="Y70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -6289,6 +6363,7 @@
       <c r="X71" t="n">
         <v>-30</v>
       </c>
+      <c r="Y71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -6371,6 +6446,7 @@
       <c r="X72" t="n">
         <v>16</v>
       </c>
+      <c r="Y72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -6453,6 +6529,7 @@
       <c r="X73" t="n">
         <v>-16</v>
       </c>
+      <c r="Y73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -6535,6 +6612,7 @@
       <c r="X74" t="n">
         <v>3</v>
       </c>
+      <c r="Y74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -6617,6 +6695,7 @@
       <c r="X75" t="n">
         <v>-3</v>
       </c>
+      <c r="Y75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -6699,6 +6778,7 @@
       <c r="X76" t="n">
         <v>-12</v>
       </c>
+      <c r="Y76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -6781,6 +6861,7 @@
       <c r="X77" t="n">
         <v>12</v>
       </c>
+      <c r="Y77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -6863,6 +6944,7 @@
       <c r="X78" t="n">
         <v>-3</v>
       </c>
+      <c r="Y78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -6945,6 +7027,7 @@
       <c r="X79" t="n">
         <v>3</v>
       </c>
+      <c r="Y79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -7027,6 +7110,7 @@
       <c r="X80" t="n">
         <v>1</v>
       </c>
+      <c r="Y80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -7109,6 +7193,7 @@
       <c r="X81" t="n">
         <v>-1</v>
       </c>
+      <c r="Y81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -7191,6 +7276,7 @@
       <c r="X82" t="n">
         <v>-8</v>
       </c>
+      <c r="Y82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -7273,6 +7359,7 @@
       <c r="X83" t="n">
         <v>8</v>
       </c>
+      <c r="Y83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -7355,6 +7442,7 @@
       <c r="X84" t="n">
         <v>40</v>
       </c>
+      <c r="Y84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -7437,6 +7525,7 @@
       <c r="X85" t="n">
         <v>-40</v>
       </c>
+      <c r="Y85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -7519,6 +7608,7 @@
       <c r="X86" t="n">
         <v>-6</v>
       </c>
+      <c r="Y86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -7601,6 +7691,7 @@
       <c r="X87" t="n">
         <v>6</v>
       </c>
+      <c r="Y87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -7683,6 +7774,7 @@
       <c r="X88" t="n">
         <v>-25</v>
       </c>
+      <c r="Y88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -7765,6 +7857,7 @@
       <c r="X89" t="n">
         <v>25</v>
       </c>
+      <c r="Y89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -7847,6 +7940,7 @@
       <c r="X90" t="n">
         <v>10</v>
       </c>
+      <c r="Y90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -7929,6 +8023,7 @@
       <c r="X91" t="n">
         <v>-10</v>
       </c>
+      <c r="Y91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -8011,6 +8106,7 @@
       <c r="X92" t="n">
         <v>-11</v>
       </c>
+      <c r="Y92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -8093,6 +8189,7 @@
       <c r="X93" t="n">
         <v>11</v>
       </c>
+      <c r="Y93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -8175,6 +8272,7 @@
       <c r="X94" t="n">
         <v>-7</v>
       </c>
+      <c r="Y94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -8257,6 +8355,7 @@
       <c r="X95" t="n">
         <v>7</v>
       </c>
+      <c r="Y95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -8339,6 +8438,7 @@
       <c r="X96" t="n">
         <v>25</v>
       </c>
+      <c r="Y96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -8421,6 +8521,7 @@
       <c r="X97" t="n">
         <v>-25</v>
       </c>
+      <c r="Y97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -8503,6 +8604,7 @@
       <c r="X98" t="n">
         <v>-5</v>
       </c>
+      <c r="Y98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -8585,6 +8687,7 @@
       <c r="X99" t="n">
         <v>5</v>
       </c>
+      <c r="Y99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -8667,6 +8770,7 @@
       <c r="X100" t="n">
         <v>-3</v>
       </c>
+      <c r="Y100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -8749,6 +8853,7 @@
       <c r="X101" t="n">
         <v>3</v>
       </c>
+      <c r="Y101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -8831,6 +8936,7 @@
       <c r="X102" t="n">
         <v>-8</v>
       </c>
+      <c r="Y102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -8913,6 +9019,7 @@
       <c r="X103" t="n">
         <v>8</v>
       </c>
+      <c r="Y103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -8995,6 +9102,7 @@
       <c r="X104" t="n">
         <v>21</v>
       </c>
+      <c r="Y104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -9077,6 +9185,7 @@
       <c r="X105" t="n">
         <v>-21</v>
       </c>
+      <c r="Y105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -9159,6 +9268,7 @@
       <c r="X106" t="n">
         <v>14</v>
       </c>
+      <c r="Y106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -9241,6 +9351,7 @@
       <c r="X107" t="n">
         <v>-14</v>
       </c>
+      <c r="Y107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -9323,6 +9434,7 @@
       <c r="X108" t="n">
         <v>-4</v>
       </c>
+      <c r="Y108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -9405,6 +9517,7 @@
       <c r="X109" t="n">
         <v>4</v>
       </c>
+      <c r="Y109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -9487,6 +9600,7 @@
       <c r="X110" t="n">
         <v>7</v>
       </c>
+      <c r="Y110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -9569,6 +9683,7 @@
       <c r="X111" t="n">
         <v>-7</v>
       </c>
+      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -9651,6 +9766,7 @@
       <c r="X112" t="n">
         <v>24</v>
       </c>
+      <c r="Y112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -9733,6 +9849,7 @@
       <c r="X113" t="n">
         <v>-24</v>
       </c>
+      <c r="Y113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -9815,6 +9932,7 @@
       <c r="X114" t="n">
         <v>-24</v>
       </c>
+      <c r="Y114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -9897,6 +10015,7 @@
       <c r="X115" t="n">
         <v>24</v>
       </c>
+      <c r="Y115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -9979,6 +10098,7 @@
       <c r="X116" t="n">
         <v>-36</v>
       </c>
+      <c r="Y116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -10061,6 +10181,7 @@
       <c r="X117" t="n">
         <v>36</v>
       </c>
+      <c r="Y117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -10143,6 +10264,7 @@
       <c r="X118" t="n">
         <v>6</v>
       </c>
+      <c r="Y118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -10225,6 +10347,7 @@
       <c r="X119" t="n">
         <v>-6</v>
       </c>
+      <c r="Y119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -10307,6 +10430,7 @@
       <c r="X120" t="n">
         <v>-7</v>
       </c>
+      <c r="Y120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -10389,6 +10513,7 @@
       <c r="X121" t="n">
         <v>7</v>
       </c>
+      <c r="Y121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -10471,6 +10596,7 @@
       <c r="X122" t="n">
         <v>18</v>
       </c>
+      <c r="Y122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -10553,6 +10679,7 @@
       <c r="X123" t="n">
         <v>-18</v>
       </c>
+      <c r="Y123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -10635,6 +10762,7 @@
       <c r="X124" t="n">
         <v>12</v>
       </c>
+      <c r="Y124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -10717,6 +10845,7 @@
       <c r="X125" t="n">
         <v>-12</v>
       </c>
+      <c r="Y125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -10799,6 +10928,7 @@
       <c r="X126" t="n">
         <v>2</v>
       </c>
+      <c r="Y126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -10881,6 +11011,7 @@
       <c r="X127" t="n">
         <v>-2</v>
       </c>
+      <c r="Y127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -10963,6 +11094,7 @@
       <c r="X128" t="n">
         <v>-5</v>
       </c>
+      <c r="Y128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -11045,6 +11177,505 @@
       <c r="X129" t="n">
         <v>5</v>
       </c>
+      <c r="Y129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2025-03-10</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>44</v>
+      </c>
+      <c r="G130" t="n">
+        <v>91</v>
+      </c>
+      <c r="H130" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="I130" t="n">
+        <v>18</v>
+      </c>
+      <c r="J130" t="n">
+        <v>42</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="L130" t="n">
+        <v>14</v>
+      </c>
+      <c r="M130" t="n">
+        <v>17</v>
+      </c>
+      <c r="N130" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="O130" t="n">
+        <v>15</v>
+      </c>
+      <c r="P130" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>43</v>
+      </c>
+      <c r="R130" t="n">
+        <v>31</v>
+      </c>
+      <c r="S130" t="n">
+        <v>9</v>
+      </c>
+      <c r="T130" t="n">
+        <v>5</v>
+      </c>
+      <c r="U130" t="n">
+        <v>19</v>
+      </c>
+      <c r="V130" t="inlineStr"/>
+      <c r="W130" t="n">
+        <v>120</v>
+      </c>
+      <c r="X130" t="n">
+        <v>-10</v>
+      </c>
+      <c r="Y130" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2025-03-10</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>45</v>
+      </c>
+      <c r="G131" t="n">
+        <v>85</v>
+      </c>
+      <c r="H131" t="n">
+        <v>0.529</v>
+      </c>
+      <c r="I131" t="n">
+        <v>21</v>
+      </c>
+      <c r="J131" t="n">
+        <v>41</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="L131" t="n">
+        <v>19</v>
+      </c>
+      <c r="M131" t="n">
+        <v>21</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="O131" t="n">
+        <v>12</v>
+      </c>
+      <c r="P131" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>40</v>
+      </c>
+      <c r="R131" t="n">
+        <v>35</v>
+      </c>
+      <c r="S131" t="n">
+        <v>16</v>
+      </c>
+      <c r="T131" t="n">
+        <v>5</v>
+      </c>
+      <c r="U131" t="n">
+        <v>17</v>
+      </c>
+      <c r="V131" t="inlineStr"/>
+      <c r="W131" t="n">
+        <v>130</v>
+      </c>
+      <c r="X131" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y131" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>37</v>
+      </c>
+      <c r="G132" t="n">
+        <v>79</v>
+      </c>
+      <c r="H132" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="I132" t="n">
+        <v>14</v>
+      </c>
+      <c r="J132" t="n">
+        <v>37</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="L132" t="n">
+        <v>16</v>
+      </c>
+      <c r="M132" t="n">
+        <v>22</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="O132" t="n">
+        <v>5</v>
+      </c>
+      <c r="P132" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q132" t="n">
+        <v>30</v>
+      </c>
+      <c r="R132" t="n">
+        <v>25</v>
+      </c>
+      <c r="S132" t="n">
+        <v>7</v>
+      </c>
+      <c r="T132" t="n">
+        <v>4</v>
+      </c>
+      <c r="U132" t="n">
+        <v>14</v>
+      </c>
+      <c r="V132" t="n">
+        <v>15</v>
+      </c>
+      <c r="W132" t="n">
+        <v>104</v>
+      </c>
+      <c r="X132" t="n">
+        <v>-26</v>
+      </c>
+      <c r="Y132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>45</v>
+      </c>
+      <c r="G133" t="n">
+        <v>78</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0.577</v>
+      </c>
+      <c r="I133" t="n">
+        <v>22</v>
+      </c>
+      <c r="J133" t="n">
+        <v>39</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.5639999999999999</v>
+      </c>
+      <c r="L133" t="n">
+        <v>18</v>
+      </c>
+      <c r="M133" t="n">
+        <v>24</v>
+      </c>
+      <c r="N133" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O133" t="n">
+        <v>7</v>
+      </c>
+      <c r="P133" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>43</v>
+      </c>
+      <c r="R133" t="n">
+        <v>35</v>
+      </c>
+      <c r="S133" t="n">
+        <v>8</v>
+      </c>
+      <c r="T133" t="n">
+        <v>5</v>
+      </c>
+      <c r="U133" t="n">
+        <v>14</v>
+      </c>
+      <c r="V133" t="n">
+        <v>21</v>
+      </c>
+      <c r="W133" t="n">
+        <v>130</v>
+      </c>
+      <c r="X133" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>NYK</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2025-03-15</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>37</v>
+      </c>
+      <c r="G134" t="n">
+        <v>86</v>
+      </c>
+      <c r="H134" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="I134" t="n">
+        <v>9</v>
+      </c>
+      <c r="J134" t="n">
+        <v>24</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="L134" t="n">
+        <v>11</v>
+      </c>
+      <c r="M134" t="n">
+        <v>13</v>
+      </c>
+      <c r="N134" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="O134" t="n">
+        <v>13</v>
+      </c>
+      <c r="P134" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q134" t="n">
+        <v>49</v>
+      </c>
+      <c r="R134" t="n">
+        <v>20</v>
+      </c>
+      <c r="S134" t="n">
+        <v>6</v>
+      </c>
+      <c r="T134" t="n">
+        <v>6</v>
+      </c>
+      <c r="U134" t="n">
+        <v>13</v>
+      </c>
+      <c r="V134" t="n">
+        <v>16</v>
+      </c>
+      <c r="W134" t="n">
+        <v>94</v>
+      </c>
+      <c r="X134" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Y134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2025-03-15</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>33</v>
+      </c>
+      <c r="G135" t="n">
+        <v>83</v>
+      </c>
+      <c r="H135" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="I135" t="n">
+        <v>13</v>
+      </c>
+      <c r="J135" t="n">
+        <v>41</v>
+      </c>
+      <c r="K135" t="n">
+        <v>0.317</v>
+      </c>
+      <c r="L135" t="n">
+        <v>18</v>
+      </c>
+      <c r="M135" t="n">
+        <v>22</v>
+      </c>
+      <c r="N135" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="O135" t="n">
+        <v>10</v>
+      </c>
+      <c r="P135" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q135" t="n">
+        <v>45</v>
+      </c>
+      <c r="R135" t="n">
+        <v>25</v>
+      </c>
+      <c r="S135" t="n">
+        <v>7</v>
+      </c>
+      <c r="T135" t="n">
+        <v>5</v>
+      </c>
+      <c r="U135" t="n">
+        <v>9</v>
+      </c>
+      <c r="V135" t="n">
+        <v>13</v>
+      </c>
+      <c r="W135" t="n">
+        <v>97</v>
+      </c>
+      <c r="X135" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y135" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix column name in json & re-run notebooks
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y135"/>
+  <dimension ref="A1:X135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,11 +549,6 @@
           <t>+/-</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>PO</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -636,7 +631,6 @@
       <c r="X2" t="n">
         <v>36</v>
       </c>
-      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -719,7 +713,6 @@
       <c r="X3" t="n">
         <v>-36</v>
       </c>
-      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -802,7 +795,6 @@
       <c r="X4" t="n">
         <v>41</v>
       </c>
-      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -885,7 +877,6 @@
       <c r="X5" t="n">
         <v>-41</v>
       </c>
-      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -968,7 +959,6 @@
       <c r="X6" t="n">
         <v>8</v>
       </c>
-      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1051,7 +1041,6 @@
       <c r="X7" t="n">
         <v>-8</v>
       </c>
-      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1134,7 +1123,6 @@
       <c r="X8" t="n">
         <v>-18</v>
       </c>
-      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1217,7 +1205,6 @@
       <c r="X9" t="n">
         <v>18</v>
       </c>
-      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1300,7 +1287,6 @@
       <c r="X10" t="n">
         <v>-15</v>
       </c>
-      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1383,7 +1369,6 @@
       <c r="X11" t="n">
         <v>15</v>
       </c>
-      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1466,7 +1451,6 @@
       <c r="X12" t="n">
         <v>6</v>
       </c>
-      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1549,7 +1533,6 @@
       <c r="X13" t="n">
         <v>-6</v>
       </c>
-      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1632,7 +1615,6 @@
       <c r="X14" t="n">
         <v>13</v>
       </c>
-      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1715,7 +1697,6 @@
       <c r="X15" t="n">
         <v>-13</v>
       </c>
-      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1798,7 +1779,6 @@
       <c r="X16" t="n">
         <v>6</v>
       </c>
-      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1881,7 +1861,6 @@
       <c r="X17" t="n">
         <v>-6</v>
       </c>
-      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1964,7 +1943,6 @@
       <c r="X18" t="n">
         <v>-19</v>
       </c>
-      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2047,7 +2025,6 @@
       <c r="X19" t="n">
         <v>19</v>
       </c>
-      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2130,7 +2107,6 @@
       <c r="X20" t="n">
         <v>11</v>
       </c>
-      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2213,7 +2189,6 @@
       <c r="X21" t="n">
         <v>-11</v>
       </c>
-      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2296,7 +2271,6 @@
       <c r="X22" t="n">
         <v>-3</v>
       </c>
-      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2379,7 +2353,6 @@
       <c r="X23" t="n">
         <v>3</v>
       </c>
-      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2462,7 +2435,6 @@
       <c r="X24" t="n">
         <v>-5</v>
       </c>
-      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2545,7 +2517,6 @@
       <c r="X25" t="n">
         <v>5</v>
       </c>
-      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2628,7 +2599,6 @@
       <c r="X26" t="n">
         <v>-3</v>
       </c>
-      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2711,7 +2681,6 @@
       <c r="X27" t="n">
         <v>3</v>
       </c>
-      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2794,7 +2763,6 @@
       <c r="X28" t="n">
         <v>-23</v>
       </c>
-      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2877,7 +2845,6 @@
       <c r="X29" t="n">
         <v>23</v>
       </c>
-      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2960,7 +2927,6 @@
       <c r="X30" t="n">
         <v>4</v>
       </c>
-      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3043,7 +3009,6 @@
       <c r="X31" t="n">
         <v>-4</v>
       </c>
-      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3126,7 +3091,6 @@
       <c r="X32" t="n">
         <v>-10</v>
       </c>
-      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3209,7 +3173,6 @@
       <c r="X33" t="n">
         <v>10</v>
       </c>
-      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -3292,7 +3255,6 @@
       <c r="X34" t="n">
         <v>8</v>
       </c>
-      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3375,7 +3337,6 @@
       <c r="X35" t="n">
         <v>-8</v>
       </c>
-      <c r="Y35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3458,7 +3419,6 @@
       <c r="X36" t="n">
         <v>4</v>
       </c>
-      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3541,7 +3501,6 @@
       <c r="X37" t="n">
         <v>-4</v>
       </c>
-      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3624,7 +3583,6 @@
       <c r="X38" t="n">
         <v>-8</v>
       </c>
-      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3707,7 +3665,6 @@
       <c r="X39" t="n">
         <v>8</v>
       </c>
-      <c r="Y39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3790,7 +3747,6 @@
       <c r="X40" t="n">
         <v>-4</v>
       </c>
-      <c r="Y40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3873,7 +3829,6 @@
       <c r="X41" t="n">
         <v>4</v>
       </c>
-      <c r="Y41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3956,7 +3911,6 @@
       <c r="X42" t="n">
         <v>-6</v>
       </c>
-      <c r="Y42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -4039,7 +3993,6 @@
       <c r="X43" t="n">
         <v>6</v>
       </c>
-      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -4122,7 +4075,6 @@
       <c r="X44" t="n">
         <v>17</v>
       </c>
-      <c r="Y44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -4205,7 +4157,6 @@
       <c r="X45" t="n">
         <v>-17</v>
       </c>
-      <c r="Y45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4288,7 +4239,6 @@
       <c r="X46" t="n">
         <v>-8</v>
       </c>
-      <c r="Y46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -4371,7 +4321,6 @@
       <c r="X47" t="n">
         <v>8</v>
       </c>
-      <c r="Y47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -4454,7 +4403,6 @@
       <c r="X48" t="n">
         <v>-1</v>
       </c>
-      <c r="Y48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4537,7 +4485,6 @@
       <c r="X49" t="n">
         <v>1</v>
       </c>
-      <c r="Y49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4620,7 +4567,6 @@
       <c r="X50" t="n">
         <v>10</v>
       </c>
-      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4703,7 +4649,6 @@
       <c r="X51" t="n">
         <v>-10</v>
       </c>
-      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4786,7 +4731,6 @@
       <c r="X52" t="n">
         <v>-51</v>
       </c>
-      <c r="Y52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -4869,7 +4813,6 @@
       <c r="X53" t="n">
         <v>51</v>
       </c>
-      <c r="Y53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -4952,7 +4895,6 @@
       <c r="X54" t="n">
         <v>10</v>
       </c>
-      <c r="Y54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -5035,7 +4977,6 @@
       <c r="X55" t="n">
         <v>-10</v>
       </c>
-      <c r="Y55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -5118,7 +5059,6 @@
       <c r="X56" t="n">
         <v>6</v>
       </c>
-      <c r="Y56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -5201,7 +5141,6 @@
       <c r="X57" t="n">
         <v>-6</v>
       </c>
-      <c r="Y57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -5284,7 +5223,6 @@
       <c r="X58" t="n">
         <v>2</v>
       </c>
-      <c r="Y58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -5367,7 +5305,6 @@
       <c r="X59" t="n">
         <v>-2</v>
       </c>
-      <c r="Y59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -5450,7 +5387,6 @@
       <c r="X60" t="n">
         <v>-10</v>
       </c>
-      <c r="Y60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -5533,7 +5469,6 @@
       <c r="X61" t="n">
         <v>10</v>
       </c>
-      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -5616,7 +5551,6 @@
       <c r="X62" t="n">
         <v>-4</v>
       </c>
-      <c r="Y62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5699,7 +5633,6 @@
       <c r="X63" t="n">
         <v>4</v>
       </c>
-      <c r="Y63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -5782,7 +5715,6 @@
       <c r="X64" t="n">
         <v>18</v>
       </c>
-      <c r="Y64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -5865,7 +5797,6 @@
       <c r="X65" t="n">
         <v>-18</v>
       </c>
-      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -5948,7 +5879,6 @@
       <c r="X66" t="n">
         <v>-34</v>
       </c>
-      <c r="Y66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -6031,7 +5961,6 @@
       <c r="X67" t="n">
         <v>34</v>
       </c>
-      <c r="Y67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -6114,7 +6043,6 @@
       <c r="X68" t="n">
         <v>-8</v>
       </c>
-      <c r="Y68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -6197,7 +6125,6 @@
       <c r="X69" t="n">
         <v>8</v>
       </c>
-      <c r="Y69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -6280,7 +6207,6 @@
       <c r="X70" t="n">
         <v>30</v>
       </c>
-      <c r="Y70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -6363,7 +6289,6 @@
       <c r="X71" t="n">
         <v>-30</v>
       </c>
-      <c r="Y71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -6446,7 +6371,6 @@
       <c r="X72" t="n">
         <v>16</v>
       </c>
-      <c r="Y72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -6529,7 +6453,6 @@
       <c r="X73" t="n">
         <v>-16</v>
       </c>
-      <c r="Y73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -6612,7 +6535,6 @@
       <c r="X74" t="n">
         <v>3</v>
       </c>
-      <c r="Y74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -6695,7 +6617,6 @@
       <c r="X75" t="n">
         <v>-3</v>
       </c>
-      <c r="Y75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -6778,7 +6699,6 @@
       <c r="X76" t="n">
         <v>-12</v>
       </c>
-      <c r="Y76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -6861,7 +6781,6 @@
       <c r="X77" t="n">
         <v>12</v>
       </c>
-      <c r="Y77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -6944,7 +6863,6 @@
       <c r="X78" t="n">
         <v>-3</v>
       </c>
-      <c r="Y78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -7027,7 +6945,6 @@
       <c r="X79" t="n">
         <v>3</v>
       </c>
-      <c r="Y79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -7110,7 +7027,6 @@
       <c r="X80" t="n">
         <v>1</v>
       </c>
-      <c r="Y80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -7193,7 +7109,6 @@
       <c r="X81" t="n">
         <v>-1</v>
       </c>
-      <c r="Y81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -7276,7 +7191,6 @@
       <c r="X82" t="n">
         <v>-8</v>
       </c>
-      <c r="Y82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -7359,7 +7273,6 @@
       <c r="X83" t="n">
         <v>8</v>
       </c>
-      <c r="Y83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -7442,7 +7355,6 @@
       <c r="X84" t="n">
         <v>40</v>
       </c>
-      <c r="Y84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -7525,7 +7437,6 @@
       <c r="X85" t="n">
         <v>-40</v>
       </c>
-      <c r="Y85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -7608,7 +7519,6 @@
       <c r="X86" t="n">
         <v>-6</v>
       </c>
-      <c r="Y86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -7691,7 +7601,6 @@
       <c r="X87" t="n">
         <v>6</v>
       </c>
-      <c r="Y87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -7774,7 +7683,6 @@
       <c r="X88" t="n">
         <v>-25</v>
       </c>
-      <c r="Y88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -7857,7 +7765,6 @@
       <c r="X89" t="n">
         <v>25</v>
       </c>
-      <c r="Y89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -7940,7 +7847,6 @@
       <c r="X90" t="n">
         <v>10</v>
       </c>
-      <c r="Y90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -8023,7 +7929,6 @@
       <c r="X91" t="n">
         <v>-10</v>
       </c>
-      <c r="Y91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -8106,7 +8011,6 @@
       <c r="X92" t="n">
         <v>-11</v>
       </c>
-      <c r="Y92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -8189,7 +8093,6 @@
       <c r="X93" t="n">
         <v>11</v>
       </c>
-      <c r="Y93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -8272,7 +8175,6 @@
       <c r="X94" t="n">
         <v>-7</v>
       </c>
-      <c r="Y94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -8355,7 +8257,6 @@
       <c r="X95" t="n">
         <v>7</v>
       </c>
-      <c r="Y95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -8438,7 +8339,6 @@
       <c r="X96" t="n">
         <v>25</v>
       </c>
-      <c r="Y96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -8521,7 +8421,6 @@
       <c r="X97" t="n">
         <v>-25</v>
       </c>
-      <c r="Y97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -8604,7 +8503,6 @@
       <c r="X98" t="n">
         <v>-5</v>
       </c>
-      <c r="Y98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -8687,7 +8585,6 @@
       <c r="X99" t="n">
         <v>5</v>
       </c>
-      <c r="Y99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -8770,7 +8667,6 @@
       <c r="X100" t="n">
         <v>-3</v>
       </c>
-      <c r="Y100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -8853,7 +8749,6 @@
       <c r="X101" t="n">
         <v>3</v>
       </c>
-      <c r="Y101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -8936,7 +8831,6 @@
       <c r="X102" t="n">
         <v>-8</v>
       </c>
-      <c r="Y102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -9019,7 +8913,6 @@
       <c r="X103" t="n">
         <v>8</v>
       </c>
-      <c r="Y103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -9102,7 +8995,6 @@
       <c r="X104" t="n">
         <v>21</v>
       </c>
-      <c r="Y104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -9185,7 +9077,6 @@
       <c r="X105" t="n">
         <v>-21</v>
       </c>
-      <c r="Y105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -9268,7 +9159,6 @@
       <c r="X106" t="n">
         <v>14</v>
       </c>
-      <c r="Y106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -9351,7 +9241,6 @@
       <c r="X107" t="n">
         <v>-14</v>
       </c>
-      <c r="Y107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -9434,7 +9323,6 @@
       <c r="X108" t="n">
         <v>-4</v>
       </c>
-      <c r="Y108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -9517,7 +9405,6 @@
       <c r="X109" t="n">
         <v>4</v>
       </c>
-      <c r="Y109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -9600,7 +9487,6 @@
       <c r="X110" t="n">
         <v>7</v>
       </c>
-      <c r="Y110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -9683,7 +9569,6 @@
       <c r="X111" t="n">
         <v>-7</v>
       </c>
-      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -9766,7 +9651,6 @@
       <c r="X112" t="n">
         <v>24</v>
       </c>
-      <c r="Y112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -9849,7 +9733,6 @@
       <c r="X113" t="n">
         <v>-24</v>
       </c>
-      <c r="Y113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -9932,7 +9815,6 @@
       <c r="X114" t="n">
         <v>-24</v>
       </c>
-      <c r="Y114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -10015,7 +9897,6 @@
       <c r="X115" t="n">
         <v>24</v>
       </c>
-      <c r="Y115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -10098,7 +9979,6 @@
       <c r="X116" t="n">
         <v>-36</v>
       </c>
-      <c r="Y116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -10181,7 +10061,6 @@
       <c r="X117" t="n">
         <v>36</v>
       </c>
-      <c r="Y117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -10264,7 +10143,6 @@
       <c r="X118" t="n">
         <v>6</v>
       </c>
-      <c r="Y118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -10347,7 +10225,6 @@
       <c r="X119" t="n">
         <v>-6</v>
       </c>
-      <c r="Y119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -10430,7 +10307,6 @@
       <c r="X120" t="n">
         <v>-7</v>
       </c>
-      <c r="Y120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -10513,7 +10389,6 @@
       <c r="X121" t="n">
         <v>7</v>
       </c>
-      <c r="Y121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -10596,7 +10471,6 @@
       <c r="X122" t="n">
         <v>18</v>
       </c>
-      <c r="Y122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -10679,7 +10553,6 @@
       <c r="X123" t="n">
         <v>-18</v>
       </c>
-      <c r="Y123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -10762,7 +10635,6 @@
       <c r="X124" t="n">
         <v>12</v>
       </c>
-      <c r="Y124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -10845,7 +10717,6 @@
       <c r="X125" t="n">
         <v>-12</v>
       </c>
-      <c r="Y125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -10928,7 +10799,6 @@
       <c r="X126" t="n">
         <v>2</v>
       </c>
-      <c r="Y126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -11011,7 +10881,6 @@
       <c r="X127" t="n">
         <v>-2</v>
       </c>
-      <c r="Y127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -11094,7 +10963,6 @@
       <c r="X128" t="n">
         <v>-5</v>
       </c>
-      <c r="Y128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -11177,7 +11045,6 @@
       <c r="X129" t="n">
         <v>5</v>
       </c>
-      <c r="Y129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -11251,15 +11118,14 @@
       <c r="U130" t="n">
         <v>19</v>
       </c>
-      <c r="V130" t="inlineStr"/>
+      <c r="V130" t="n">
+        <v>13</v>
+      </c>
       <c r="W130" t="n">
         <v>120</v>
       </c>
       <c r="X130" t="n">
         <v>-10</v>
-      </c>
-      <c r="Y130" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="131">
@@ -11334,15 +11200,14 @@
       <c r="U131" t="n">
         <v>17</v>
       </c>
-      <c r="V131" t="inlineStr"/>
+      <c r="V131" t="n">
+        <v>16</v>
+      </c>
       <c r="W131" t="n">
         <v>130</v>
       </c>
       <c r="X131" t="n">
         <v>10</v>
-      </c>
-      <c r="Y131" t="n">
-        <v>16</v>
       </c>
     </row>
     <row r="132">
@@ -11426,7 +11291,6 @@
       <c r="X132" t="n">
         <v>-26</v>
       </c>
-      <c r="Y132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -11509,7 +11373,6 @@
       <c r="X133" t="n">
         <v>26</v>
       </c>
-      <c r="Y133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -11592,7 +11455,6 @@
       <c r="X134" t="n">
         <v>-3</v>
       </c>
-      <c r="Y134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -11675,7 +11537,6 @@
       <c r="X135" t="n">
         <v>3</v>
       </c>
-      <c r="Y135" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update json box scores & re-run spreadsheet-creation script
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y135"/>
+  <dimension ref="A1:Y143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12213,6 +12213,702 @@
         <v>3</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>2025-03-17</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>43</v>
+      </c>
+      <c r="H136" t="n">
+        <v>92</v>
+      </c>
+      <c r="I136" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="J136" t="n">
+        <v>14</v>
+      </c>
+      <c r="K136" t="n">
+        <v>39</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0.359</v>
+      </c>
+      <c r="M136" t="n">
+        <v>14</v>
+      </c>
+      <c r="N136" t="n">
+        <v>18</v>
+      </c>
+      <c r="O136" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="P136" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q136" t="n">
+        <v>34</v>
+      </c>
+      <c r="R136" t="n">
+        <v>53</v>
+      </c>
+      <c r="S136" t="n">
+        <v>32</v>
+      </c>
+      <c r="T136" t="n">
+        <v>12</v>
+      </c>
+      <c r="U136" t="n">
+        <v>7</v>
+      </c>
+      <c r="V136" t="n">
+        <v>20</v>
+      </c>
+      <c r="W136" t="n">
+        <v>24</v>
+      </c>
+      <c r="X136" t="n">
+        <v>114</v>
+      </c>
+      <c r="Y136" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>2025-03-17</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>41</v>
+      </c>
+      <c r="H137" t="n">
+        <v>84</v>
+      </c>
+      <c r="I137" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="J137" t="n">
+        <v>8</v>
+      </c>
+      <c r="K137" t="n">
+        <v>33</v>
+      </c>
+      <c r="L137" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="M137" t="n">
+        <v>15</v>
+      </c>
+      <c r="N137" t="n">
+        <v>27</v>
+      </c>
+      <c r="O137" t="n">
+        <v>0.556</v>
+      </c>
+      <c r="P137" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q137" t="n">
+        <v>27</v>
+      </c>
+      <c r="R137" t="n">
+        <v>38</v>
+      </c>
+      <c r="S137" t="n">
+        <v>24</v>
+      </c>
+      <c r="T137" t="n">
+        <v>16</v>
+      </c>
+      <c r="U137" t="n">
+        <v>10</v>
+      </c>
+      <c r="V137" t="n">
+        <v>20</v>
+      </c>
+      <c r="W137" t="n">
+        <v>21</v>
+      </c>
+      <c r="X137" t="n">
+        <v>105</v>
+      </c>
+      <c r="Y137" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>31</v>
+      </c>
+      <c r="H138" t="n">
+        <v>79</v>
+      </c>
+      <c r="I138" t="n">
+        <v>0.392</v>
+      </c>
+      <c r="J138" t="n">
+        <v>12</v>
+      </c>
+      <c r="K138" t="n">
+        <v>38</v>
+      </c>
+      <c r="L138" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="M138" t="n">
+        <v>19</v>
+      </c>
+      <c r="N138" t="n">
+        <v>27</v>
+      </c>
+      <c r="O138" t="n">
+        <v>0.704</v>
+      </c>
+      <c r="P138" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>30</v>
+      </c>
+      <c r="R138" t="n">
+        <v>34</v>
+      </c>
+      <c r="S138" t="n">
+        <v>19</v>
+      </c>
+      <c r="T138" t="n">
+        <v>9</v>
+      </c>
+      <c r="U138" t="n">
+        <v>4</v>
+      </c>
+      <c r="V138" t="n">
+        <v>9</v>
+      </c>
+      <c r="W138" t="n">
+        <v>15</v>
+      </c>
+      <c r="X138" t="n">
+        <v>93</v>
+      </c>
+      <c r="Y138" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>32</v>
+      </c>
+      <c r="H139" t="n">
+        <v>77</v>
+      </c>
+      <c r="I139" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="J139" t="n">
+        <v>17</v>
+      </c>
+      <c r="K139" t="n">
+        <v>44</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="M139" t="n">
+        <v>23</v>
+      </c>
+      <c r="N139" t="n">
+        <v>26</v>
+      </c>
+      <c r="O139" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="P139" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>43</v>
+      </c>
+      <c r="R139" t="n">
+        <v>52</v>
+      </c>
+      <c r="S139" t="n">
+        <v>25</v>
+      </c>
+      <c r="T139" t="n">
+        <v>7</v>
+      </c>
+      <c r="U139" t="n">
+        <v>6</v>
+      </c>
+      <c r="V139" t="n">
+        <v>18</v>
+      </c>
+      <c r="W139" t="n">
+        <v>24</v>
+      </c>
+      <c r="X139" t="n">
+        <v>104</v>
+      </c>
+      <c r="Y139" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>2025-03-20</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>44</v>
+      </c>
+      <c r="H140" t="n">
+        <v>78</v>
+      </c>
+      <c r="I140" t="n">
+        <v>0.5639999999999999</v>
+      </c>
+      <c r="J140" t="n">
+        <v>11</v>
+      </c>
+      <c r="K140" t="n">
+        <v>26</v>
+      </c>
+      <c r="L140" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="M140" t="n">
+        <v>15</v>
+      </c>
+      <c r="N140" t="n">
+        <v>19</v>
+      </c>
+      <c r="O140" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="P140" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>37</v>
+      </c>
+      <c r="R140" t="n">
+        <v>44</v>
+      </c>
+      <c r="S140" t="n">
+        <v>32</v>
+      </c>
+      <c r="T140" t="n">
+        <v>7</v>
+      </c>
+      <c r="U140" t="n">
+        <v>4</v>
+      </c>
+      <c r="V140" t="n">
+        <v>23</v>
+      </c>
+      <c r="W140" t="n">
+        <v>24</v>
+      </c>
+      <c r="X140" t="n">
+        <v>114</v>
+      </c>
+      <c r="Y140" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>2025-03-20</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>38</v>
+      </c>
+      <c r="H141" t="n">
+        <v>90</v>
+      </c>
+      <c r="I141" t="n">
+        <v>0.422</v>
+      </c>
+      <c r="J141" t="n">
+        <v>19</v>
+      </c>
+      <c r="K141" t="n">
+        <v>47</v>
+      </c>
+      <c r="L141" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="M141" t="n">
+        <v>22</v>
+      </c>
+      <c r="N141" t="n">
+        <v>28</v>
+      </c>
+      <c r="O141" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="P141" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q141" t="n">
+        <v>27</v>
+      </c>
+      <c r="R141" t="n">
+        <v>38</v>
+      </c>
+      <c r="S141" t="n">
+        <v>30</v>
+      </c>
+      <c r="T141" t="n">
+        <v>13</v>
+      </c>
+      <c r="U141" t="n">
+        <v>5</v>
+      </c>
+      <c r="V141" t="n">
+        <v>14</v>
+      </c>
+      <c r="W141" t="n">
+        <v>15</v>
+      </c>
+      <c r="X141" t="n">
+        <v>117</v>
+      </c>
+      <c r="Y141" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>39</v>
+      </c>
+      <c r="H142" t="n">
+        <v>84</v>
+      </c>
+      <c r="I142" t="n">
+        <v>0.464</v>
+      </c>
+      <c r="J142" t="n">
+        <v>16</v>
+      </c>
+      <c r="K142" t="n">
+        <v>38</v>
+      </c>
+      <c r="L142" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="M142" t="n">
+        <v>21</v>
+      </c>
+      <c r="N142" t="n">
+        <v>26</v>
+      </c>
+      <c r="O142" t="n">
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="P142" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q142" t="n">
+        <v>32</v>
+      </c>
+      <c r="R142" t="n">
+        <v>38</v>
+      </c>
+      <c r="S142" t="n">
+        <v>28</v>
+      </c>
+      <c r="T142" t="n">
+        <v>8</v>
+      </c>
+      <c r="U142" t="n">
+        <v>4</v>
+      </c>
+      <c r="V142" t="n">
+        <v>9</v>
+      </c>
+      <c r="W142" t="n">
+        <v>16</v>
+      </c>
+      <c r="X142" t="n">
+        <v>115</v>
+      </c>
+      <c r="Y142" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>49</v>
+      </c>
+      <c r="H143" t="n">
+        <v>86</v>
+      </c>
+      <c r="I143" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="J143" t="n">
+        <v>15</v>
+      </c>
+      <c r="K143" t="n">
+        <v>36</v>
+      </c>
+      <c r="L143" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="M143" t="n">
+        <v>11</v>
+      </c>
+      <c r="N143" t="n">
+        <v>18</v>
+      </c>
+      <c r="O143" t="n">
+        <v>0.611</v>
+      </c>
+      <c r="P143" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q143" t="n">
+        <v>36</v>
+      </c>
+      <c r="R143" t="n">
+        <v>46</v>
+      </c>
+      <c r="S143" t="n">
+        <v>37</v>
+      </c>
+      <c r="T143" t="n">
+        <v>5</v>
+      </c>
+      <c r="U143" t="n">
+        <v>3</v>
+      </c>
+      <c r="V143" t="n">
+        <v>14</v>
+      </c>
+      <c r="W143" t="n">
+        <v>23</v>
+      </c>
+      <c r="X143" t="n">
+        <v>124</v>
+      </c>
+      <c r="Y143" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add latest GSW box scores & re-run GSW notebooks
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y143"/>
+  <dimension ref="A1:Y147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12909,6 +12909,354 @@
         <v>9</v>
       </c>
     </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>33</v>
+      </c>
+      <c r="H144" t="n">
+        <v>83</v>
+      </c>
+      <c r="I144" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="J144" t="n">
+        <v>9</v>
+      </c>
+      <c r="K144" t="n">
+        <v>38</v>
+      </c>
+      <c r="L144" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="M144" t="n">
+        <v>11</v>
+      </c>
+      <c r="N144" t="n">
+        <v>16</v>
+      </c>
+      <c r="O144" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="P144" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q144" t="n">
+        <v>24</v>
+      </c>
+      <c r="R144" t="n">
+        <v>38</v>
+      </c>
+      <c r="S144" t="n">
+        <v>20</v>
+      </c>
+      <c r="T144" t="n">
+        <v>8</v>
+      </c>
+      <c r="U144" t="n">
+        <v>1</v>
+      </c>
+      <c r="V144" t="n">
+        <v>12</v>
+      </c>
+      <c r="W144" t="n">
+        <v>14</v>
+      </c>
+      <c r="X144" t="n">
+        <v>86</v>
+      </c>
+      <c r="Y144" t="n">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>43</v>
+      </c>
+      <c r="H145" t="n">
+        <v>77</v>
+      </c>
+      <c r="I145" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="J145" t="n">
+        <v>17</v>
+      </c>
+      <c r="K145" t="n">
+        <v>25</v>
+      </c>
+      <c r="L145" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="M145" t="n">
+        <v>9</v>
+      </c>
+      <c r="N145" t="n">
+        <v>12</v>
+      </c>
+      <c r="O145" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="P145" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q145" t="n">
+        <v>34</v>
+      </c>
+      <c r="R145" t="n">
+        <v>42</v>
+      </c>
+      <c r="S145" t="n">
+        <v>26</v>
+      </c>
+      <c r="T145" t="n">
+        <v>8</v>
+      </c>
+      <c r="U145" t="n">
+        <v>5</v>
+      </c>
+      <c r="V145" t="n">
+        <v>15</v>
+      </c>
+      <c r="W145" t="n">
+        <v>15</v>
+      </c>
+      <c r="X145" t="n">
+        <v>112</v>
+      </c>
+      <c r="Y145" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>NOP</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>2025-03-28</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>38</v>
+      </c>
+      <c r="H146" t="n">
+        <v>92</v>
+      </c>
+      <c r="I146" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="J146" t="n">
+        <v>13</v>
+      </c>
+      <c r="K146" t="n">
+        <v>55</v>
+      </c>
+      <c r="L146" t="n">
+        <v>0.236</v>
+      </c>
+      <c r="M146" t="n">
+        <v>22</v>
+      </c>
+      <c r="N146" t="n">
+        <v>29</v>
+      </c>
+      <c r="O146" t="n">
+        <v>0.759</v>
+      </c>
+      <c r="P146" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>32</v>
+      </c>
+      <c r="R146" t="n">
+        <v>50</v>
+      </c>
+      <c r="S146" t="n">
+        <v>29</v>
+      </c>
+      <c r="T146" t="n">
+        <v>10</v>
+      </c>
+      <c r="U146" t="n">
+        <v>1</v>
+      </c>
+      <c r="V146" t="n">
+        <v>10</v>
+      </c>
+      <c r="W146" t="n">
+        <v>22</v>
+      </c>
+      <c r="X146" t="n">
+        <v>111</v>
+      </c>
+      <c r="Y146" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>NOP</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>2025-03-28</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>33</v>
+      </c>
+      <c r="H147" t="n">
+        <v>81</v>
+      </c>
+      <c r="I147" t="n">
+        <v>0.407</v>
+      </c>
+      <c r="J147" t="n">
+        <v>7</v>
+      </c>
+      <c r="K147" t="n">
+        <v>23</v>
+      </c>
+      <c r="L147" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="M147" t="n">
+        <v>22</v>
+      </c>
+      <c r="N147" t="n">
+        <v>28</v>
+      </c>
+      <c r="O147" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="P147" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q147" t="n">
+        <v>32</v>
+      </c>
+      <c r="R147" t="n">
+        <v>46</v>
+      </c>
+      <c r="S147" t="n">
+        <v>24</v>
+      </c>
+      <c r="T147" t="n">
+        <v>6</v>
+      </c>
+      <c r="U147" t="n">
+        <v>5</v>
+      </c>
+      <c r="V147" t="n">
+        <v>15</v>
+      </c>
+      <c r="W147" t="n">
+        <v>23</v>
+      </c>
+      <c r="X147" t="n">
+        <v>95</v>
+      </c>
+      <c r="Y147" t="n">
+        <v>-16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add W/L & points per quarter columns to GSW team box scores
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y147"/>
+  <dimension ref="A1:AD147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,31 @@
           <t>+/-</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Q3</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>W/L</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -641,6 +666,23 @@
       <c r="Y2" t="n">
         <v>36</v>
       </c>
+      <c r="Z2" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>41</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>40</v>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -728,6 +770,23 @@
       <c r="Y3" t="n">
         <v>-36</v>
       </c>
+      <c r="Z3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -815,6 +874,23 @@
       <c r="Y4" t="n">
         <v>41</v>
       </c>
+      <c r="Z4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -902,6 +978,23 @@
       <c r="Y5" t="n">
         <v>-41</v>
       </c>
+      <c r="Z5" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -989,6 +1082,23 @@
       <c r="Y6" t="n">
         <v>8</v>
       </c>
+      <c r="Z6" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1076,6 +1186,23 @@
       <c r="Y7" t="n">
         <v>-8</v>
       </c>
+      <c r="Z7" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1163,6 +1290,23 @@
       <c r="Y8" t="n">
         <v>-18</v>
       </c>
+      <c r="Z8" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1250,6 +1394,23 @@
       <c r="Y9" t="n">
         <v>18</v>
       </c>
+      <c r="Z9" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1337,6 +1498,23 @@
       <c r="Y10" t="n">
         <v>-15</v>
       </c>
+      <c r="Z10" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1424,6 +1602,23 @@
       <c r="Y11" t="n">
         <v>15</v>
       </c>
+      <c r="Z11" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1511,6 +1706,23 @@
       <c r="Y12" t="n">
         <v>6</v>
       </c>
+      <c r="Z12" t="n">
+        <v>38</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1598,6 +1810,23 @@
       <c r="Y13" t="n">
         <v>-6</v>
       </c>
+      <c r="Z13" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>39</v>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1685,6 +1914,23 @@
       <c r="Y14" t="n">
         <v>13</v>
       </c>
+      <c r="Z14" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1772,6 +2018,23 @@
       <c r="Y15" t="n">
         <v>-13</v>
       </c>
+      <c r="Z15" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1859,6 +2122,23 @@
       <c r="Y16" t="n">
         <v>6</v>
       </c>
+      <c r="Z16" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>36</v>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1946,6 +2226,23 @@
       <c r="Y17" t="n">
         <v>-6</v>
       </c>
+      <c r="Z17" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>16</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>41</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2033,6 +2330,23 @@
       <c r="Y18" t="n">
         <v>-19</v>
       </c>
+      <c r="Z18" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>41</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>34</v>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2120,6 +2434,23 @@
       <c r="Y19" t="n">
         <v>19</v>
       </c>
+      <c r="Z19" t="n">
+        <v>39</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>44</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2207,6 +2538,23 @@
       <c r="Y20" t="n">
         <v>11</v>
       </c>
+      <c r="Z20" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>39</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2294,6 +2642,23 @@
       <c r="Y21" t="n">
         <v>-11</v>
       </c>
+      <c r="Z21" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2381,6 +2746,23 @@
       <c r="Y22" t="n">
         <v>-3</v>
       </c>
+      <c r="Z22" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>36</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2468,6 +2850,23 @@
       <c r="Y23" t="n">
         <v>3</v>
       </c>
+      <c r="Z23" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2555,6 +2954,23 @@
       <c r="Y24" t="n">
         <v>-5</v>
       </c>
+      <c r="Z24" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>40</v>
+      </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2642,6 +3058,23 @@
       <c r="Y25" t="n">
         <v>5</v>
       </c>
+      <c r="Z25" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2729,6 +3162,23 @@
       <c r="Y26" t="n">
         <v>-3</v>
       </c>
+      <c r="Z26" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2816,6 +3266,23 @@
       <c r="Y27" t="n">
         <v>3</v>
       </c>
+      <c r="Z27" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2903,6 +3370,23 @@
       <c r="Y28" t="n">
         <v>-23</v>
       </c>
+      <c r="Z28" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2990,6 +3474,23 @@
       <c r="Y29" t="n">
         <v>23</v>
       </c>
+      <c r="Z29" t="n">
+        <v>41</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -3077,6 +3578,23 @@
       <c r="Y30" t="n">
         <v>4</v>
       </c>
+      <c r="Z30" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3164,6 +3682,23 @@
       <c r="Y31" t="n">
         <v>-4</v>
       </c>
+      <c r="Z31" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3251,6 +3786,23 @@
       <c r="Y32" t="n">
         <v>-10</v>
       </c>
+      <c r="Z32" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3338,6 +3890,23 @@
       <c r="Y33" t="n">
         <v>10</v>
       </c>
+      <c r="Z33" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -3425,6 +3994,23 @@
       <c r="Y34" t="n">
         <v>8</v>
       </c>
+      <c r="Z34" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>41</v>
+      </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3512,6 +4098,23 @@
       <c r="Y35" t="n">
         <v>-8</v>
       </c>
+      <c r="Z35" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>37</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3599,6 +4202,23 @@
       <c r="Y36" t="n">
         <v>4</v>
       </c>
+      <c r="Z36" t="n">
+        <v>39</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD36" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3686,6 +4306,23 @@
       <c r="Y37" t="n">
         <v>-4</v>
       </c>
+      <c r="Z37" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC37" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD37" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3773,6 +4410,23 @@
       <c r="Y38" t="n">
         <v>-8</v>
       </c>
+      <c r="Z38" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD38" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3860,6 +4514,23 @@
       <c r="Y39" t="n">
         <v>8</v>
       </c>
+      <c r="Z39" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>31</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD39" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3947,6 +4618,23 @@
       <c r="Y40" t="n">
         <v>-4</v>
       </c>
+      <c r="Z40" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC40" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD40" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -4034,6 +4722,23 @@
       <c r="Y41" t="n">
         <v>4</v>
       </c>
+      <c r="Z41" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC41" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD41" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -4121,6 +4826,23 @@
       <c r="Y42" t="n">
         <v>-6</v>
       </c>
+      <c r="Z42" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB42" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC42" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD42" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -4208,6 +4930,23 @@
       <c r="Y43" t="n">
         <v>6</v>
       </c>
+      <c r="Z43" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>31</v>
+      </c>
+      <c r="AB43" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC43" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD43" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -4295,6 +5034,23 @@
       <c r="Y44" t="n">
         <v>17</v>
       </c>
+      <c r="Z44" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB44" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC44" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD44" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -4382,6 +5138,23 @@
       <c r="Y45" t="n">
         <v>-17</v>
       </c>
+      <c r="Z45" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>15</v>
+      </c>
+      <c r="AB45" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC45" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4469,6 +5242,23 @@
       <c r="Y46" t="n">
         <v>-8</v>
       </c>
+      <c r="Z46" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB46" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC46" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -4556,6 +5346,23 @@
       <c r="Y47" t="n">
         <v>8</v>
       </c>
+      <c r="Z47" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB47" t="n">
+        <v>44</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD47" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -4643,6 +5450,23 @@
       <c r="Y48" t="n">
         <v>-1</v>
       </c>
+      <c r="Z48" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>19</v>
+      </c>
+      <c r="AB48" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC48" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD48" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4730,6 +5554,23 @@
       <c r="Y49" t="n">
         <v>1</v>
       </c>
+      <c r="Z49" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB49" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC49" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD49" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4817,6 +5658,23 @@
       <c r="Y50" t="n">
         <v>10</v>
       </c>
+      <c r="Z50" t="n">
+        <v>46</v>
+      </c>
+      <c r="AA50" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB50" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC50" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4904,6 +5762,23 @@
       <c r="Y51" t="n">
         <v>-10</v>
       </c>
+      <c r="Z51" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>41</v>
+      </c>
+      <c r="AB51" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC51" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4991,6 +5866,23 @@
       <c r="Y52" t="n">
         <v>-51</v>
       </c>
+      <c r="Z52" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB52" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC52" t="n">
+        <v>34</v>
+      </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -5078,6 +5970,23 @@
       <c r="Y53" t="n">
         <v>51</v>
       </c>
+      <c r="Z53" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB53" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC53" t="n">
+        <v>35</v>
+      </c>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -5165,6 +6074,23 @@
       <c r="Y54" t="n">
         <v>10</v>
       </c>
+      <c r="Z54" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB54" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC54" t="n">
+        <v>34</v>
+      </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -5252,6 +6178,23 @@
       <c r="Y55" t="n">
         <v>-10</v>
       </c>
+      <c r="Z55" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB55" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC55" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -5339,6 +6282,23 @@
       <c r="Y56" t="n">
         <v>6</v>
       </c>
+      <c r="Z56" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB56" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC56" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -5426,6 +6386,23 @@
       <c r="Y57" t="n">
         <v>-6</v>
       </c>
+      <c r="Z57" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB57" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC57" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -5513,6 +6490,23 @@
       <c r="Y58" t="n">
         <v>2</v>
       </c>
+      <c r="Z58" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB58" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC58" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -5600,6 +6594,23 @@
       <c r="Y59" t="n">
         <v>-2</v>
       </c>
+      <c r="Z59" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB59" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC59" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -5687,6 +6698,23 @@
       <c r="Y60" t="n">
         <v>-10</v>
       </c>
+      <c r="Z60" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB60" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC60" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -5774,6 +6802,23 @@
       <c r="Y61" t="n">
         <v>10</v>
       </c>
+      <c r="Z61" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB61" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC61" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -5861,6 +6906,23 @@
       <c r="Y62" t="n">
         <v>-4</v>
       </c>
+      <c r="Z62" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA62" t="n">
+        <v>38</v>
+      </c>
+      <c r="AB62" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC62" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5948,6 +7010,23 @@
       <c r="Y63" t="n">
         <v>4</v>
       </c>
+      <c r="Z63" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA63" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB63" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC63" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD63" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -6035,6 +7114,23 @@
       <c r="Y64" t="n">
         <v>18</v>
       </c>
+      <c r="Z64" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA64" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB64" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC64" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD64" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -6122,6 +7218,23 @@
       <c r="Y65" t="n">
         <v>-18</v>
       </c>
+      <c r="Z65" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA65" t="n">
+        <v>11</v>
+      </c>
+      <c r="AB65" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC65" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD65" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -6209,6 +7322,23 @@
       <c r="Y66" t="n">
         <v>-34</v>
       </c>
+      <c r="Z66" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA66" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB66" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC66" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD66" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -6296,6 +7426,23 @@
       <c r="Y67" t="n">
         <v>34</v>
       </c>
+      <c r="Z67" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA67" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB67" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC67" t="n">
+        <v>36</v>
+      </c>
+      <c r="AD67" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -6383,6 +7530,23 @@
       <c r="Y68" t="n">
         <v>-8</v>
       </c>
+      <c r="Z68" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA68" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB68" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC68" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD68" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -6470,6 +7634,23 @@
       <c r="Y69" t="n">
         <v>8</v>
       </c>
+      <c r="Z69" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA69" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB69" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC69" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD69" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -6557,6 +7738,23 @@
       <c r="Y70" t="n">
         <v>30</v>
       </c>
+      <c r="Z70" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA70" t="n">
+        <v>39</v>
+      </c>
+      <c r="AB70" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC70" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD70" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -6644,6 +7842,23 @@
       <c r="Y71" t="n">
         <v>-30</v>
       </c>
+      <c r="Z71" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB71" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC71" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD71" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -6731,6 +7946,23 @@
       <c r="Y72" t="n">
         <v>16</v>
       </c>
+      <c r="Z72" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA72" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB72" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC72" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD72" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -6818,6 +8050,23 @@
       <c r="Y73" t="n">
         <v>-16</v>
       </c>
+      <c r="Z73" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA73" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB73" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC73" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD73" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -6905,6 +8154,23 @@
       <c r="Y74" t="n">
         <v>3</v>
       </c>
+      <c r="Z74" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA74" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB74" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC74" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD74" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -6992,6 +8258,23 @@
       <c r="Y75" t="n">
         <v>-3</v>
       </c>
+      <c r="Z75" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA75" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB75" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC75" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD75" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -7079,6 +8362,23 @@
       <c r="Y76" t="n">
         <v>-12</v>
       </c>
+      <c r="Z76" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA76" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB76" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC76" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD76" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -7166,6 +8466,23 @@
       <c r="Y77" t="n">
         <v>12</v>
       </c>
+      <c r="Z77" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA77" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB77" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC77" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD77" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -7253,6 +8570,23 @@
       <c r="Y78" t="n">
         <v>-3</v>
       </c>
+      <c r="Z78" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA78" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB78" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC78" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD78" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -7340,6 +8674,23 @@
       <c r="Y79" t="n">
         <v>3</v>
       </c>
+      <c r="Z79" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA79" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB79" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC79" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD79" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -7427,6 +8778,23 @@
       <c r="Y80" t="n">
         <v>1</v>
       </c>
+      <c r="Z80" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA80" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB80" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC80" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD80" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -7514,6 +8882,23 @@
       <c r="Y81" t="n">
         <v>-1</v>
       </c>
+      <c r="Z81" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA81" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB81" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC81" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD81" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -7601,6 +8986,23 @@
       <c r="Y82" t="n">
         <v>-8</v>
       </c>
+      <c r="Z82" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA82" t="n">
+        <v>31</v>
+      </c>
+      <c r="AB82" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC82" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD82" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -7688,6 +9090,23 @@
       <c r="Y83" t="n">
         <v>8</v>
       </c>
+      <c r="Z83" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA83" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB83" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC83" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD83" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -7775,6 +9194,23 @@
       <c r="Y84" t="n">
         <v>40</v>
       </c>
+      <c r="Z84" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA84" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB84" t="n">
+        <v>43</v>
+      </c>
+      <c r="AC84" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD84" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -7862,6 +9298,23 @@
       <c r="Y85" t="n">
         <v>-40</v>
       </c>
+      <c r="Z85" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA85" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB85" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC85" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD85" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -7949,6 +9402,23 @@
       <c r="Y86" t="n">
         <v>-6</v>
       </c>
+      <c r="Z86" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA86" t="n">
+        <v>41</v>
+      </c>
+      <c r="AB86" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC86" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD86" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -8036,6 +9506,23 @@
       <c r="Y87" t="n">
         <v>6</v>
       </c>
+      <c r="Z87" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA87" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB87" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC87" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD87" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -8123,6 +9610,23 @@
       <c r="Y88" t="n">
         <v>-25</v>
       </c>
+      <c r="Z88" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA88" t="n">
+        <v>31</v>
+      </c>
+      <c r="AB88" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC88" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD88" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -8210,6 +9714,23 @@
       <c r="Y89" t="n">
         <v>25</v>
       </c>
+      <c r="Z89" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA89" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB89" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC89" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD89" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -8297,6 +9818,23 @@
       <c r="Y90" t="n">
         <v>10</v>
       </c>
+      <c r="Z90" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA90" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB90" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC90" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD90" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -8384,6 +9922,23 @@
       <c r="Y91" t="n">
         <v>-10</v>
       </c>
+      <c r="Z91" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA91" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB91" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC91" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD91" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -8471,6 +10026,23 @@
       <c r="Y92" t="n">
         <v>-11</v>
       </c>
+      <c r="Z92" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA92" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB92" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC92" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD92" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -8558,6 +10130,23 @@
       <c r="Y93" t="n">
         <v>11</v>
       </c>
+      <c r="Z93" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA93" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB93" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC93" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD93" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -8645,6 +10234,23 @@
       <c r="Y94" t="n">
         <v>-7</v>
       </c>
+      <c r="Z94" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA94" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB94" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC94" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD94" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -8732,6 +10338,23 @@
       <c r="Y95" t="n">
         <v>7</v>
       </c>
+      <c r="Z95" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA95" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB95" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC95" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD95" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -8819,6 +10442,23 @@
       <c r="Y96" t="n">
         <v>25</v>
       </c>
+      <c r="Z96" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA96" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB96" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC96" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD96" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -8906,6 +10546,23 @@
       <c r="Y97" t="n">
         <v>-25</v>
       </c>
+      <c r="Z97" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA97" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB97" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC97" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD97" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -8993,6 +10650,23 @@
       <c r="Y98" t="n">
         <v>-5</v>
       </c>
+      <c r="Z98" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA98" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB98" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC98" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD98" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -9080,6 +10754,23 @@
       <c r="Y99" t="n">
         <v>5</v>
       </c>
+      <c r="Z99" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA99" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB99" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC99" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD99" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -9167,6 +10858,23 @@
       <c r="Y100" t="n">
         <v>-3</v>
       </c>
+      <c r="Z100" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA100" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB100" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC100" t="n">
+        <v>41</v>
+      </c>
+      <c r="AD100" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -9254,6 +10962,23 @@
       <c r="Y101" t="n">
         <v>3</v>
       </c>
+      <c r="Z101" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA101" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB101" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC101" t="n">
+        <v>44</v>
+      </c>
+      <c r="AD101" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -9341,6 +11066,23 @@
       <c r="Y102" t="n">
         <v>-8</v>
       </c>
+      <c r="Z102" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA102" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB102" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC102" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD102" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -9428,6 +11170,23 @@
       <c r="Y103" t="n">
         <v>8</v>
       </c>
+      <c r="Z103" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA103" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB103" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC103" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD103" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -9515,6 +11274,23 @@
       <c r="Y104" t="n">
         <v>21</v>
       </c>
+      <c r="Z104" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA104" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB104" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC104" t="n">
+        <v>35</v>
+      </c>
+      <c r="AD104" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -9602,6 +11378,23 @@
       <c r="Y105" t="n">
         <v>-21</v>
       </c>
+      <c r="Z105" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA105" t="n">
+        <v>38</v>
+      </c>
+      <c r="AB105" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC105" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD105" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -9689,6 +11482,23 @@
       <c r="Y106" t="n">
         <v>14</v>
       </c>
+      <c r="Z106" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA106" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB106" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC106" t="n">
+        <v>36</v>
+      </c>
+      <c r="AD106" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -9776,6 +11586,23 @@
       <c r="Y107" t="n">
         <v>-14</v>
       </c>
+      <c r="Z107" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA107" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB107" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC107" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD107" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -9863,6 +11690,23 @@
       <c r="Y108" t="n">
         <v>-4</v>
       </c>
+      <c r="Z108" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA108" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB108" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC108" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD108" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -9950,6 +11794,23 @@
       <c r="Y109" t="n">
         <v>4</v>
       </c>
+      <c r="Z109" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA109" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB109" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC109" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD109" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -10037,6 +11898,23 @@
       <c r="Y110" t="n">
         <v>7</v>
       </c>
+      <c r="Z110" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA110" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB110" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC110" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD110" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -10124,6 +12002,23 @@
       <c r="Y111" t="n">
         <v>-7</v>
       </c>
+      <c r="Z111" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA111" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB111" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC111" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD111" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -10211,6 +12106,23 @@
       <c r="Y112" t="n">
         <v>24</v>
       </c>
+      <c r="Z112" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA112" t="n">
+        <v>37</v>
+      </c>
+      <c r="AB112" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC112" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD112" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -10298,6 +12210,23 @@
       <c r="Y113" t="n">
         <v>-24</v>
       </c>
+      <c r="Z113" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA113" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB113" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC113" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD113" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -10385,6 +12314,23 @@
       <c r="Y114" t="n">
         <v>-24</v>
       </c>
+      <c r="Z114" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA114" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB114" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC114" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD114" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -10472,6 +12418,23 @@
       <c r="Y115" t="n">
         <v>24</v>
       </c>
+      <c r="Z115" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA115" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB115" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC115" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD115" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -10559,6 +12522,23 @@
       <c r="Y116" t="n">
         <v>-36</v>
       </c>
+      <c r="Z116" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA116" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB116" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC116" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD116" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -10646,6 +12626,23 @@
       <c r="Y117" t="n">
         <v>36</v>
       </c>
+      <c r="Z117" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA117" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB117" t="n">
+        <v>41</v>
+      </c>
+      <c r="AC117" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD117" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -10733,6 +12730,23 @@
       <c r="Y118" t="n">
         <v>6</v>
       </c>
+      <c r="Z118" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA118" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB118" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC118" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD118" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -10820,6 +12834,23 @@
       <c r="Y119" t="n">
         <v>-6</v>
       </c>
+      <c r="Z119" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA119" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB119" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC119" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD119" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -10907,6 +12938,23 @@
       <c r="Y120" t="n">
         <v>-7</v>
       </c>
+      <c r="Z120" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA120" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB120" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC120" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD120" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -10994,6 +13042,23 @@
       <c r="Y121" t="n">
         <v>7</v>
       </c>
+      <c r="Z121" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA121" t="n">
+        <v>37</v>
+      </c>
+      <c r="AB121" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC121" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD121" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -11081,6 +13146,23 @@
       <c r="Y122" t="n">
         <v>18</v>
       </c>
+      <c r="Z122" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA122" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB122" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC122" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD122" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -11168,6 +13250,23 @@
       <c r="Y123" t="n">
         <v>-18</v>
       </c>
+      <c r="Z123" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA123" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB123" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC123" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD123" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -11255,6 +13354,23 @@
       <c r="Y124" t="n">
         <v>12</v>
       </c>
+      <c r="Z124" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA124" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB124" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC124" t="n">
+        <v>32</v>
+      </c>
+      <c r="AD124" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -11342,6 +13458,23 @@
       <c r="Y125" t="n">
         <v>-12</v>
       </c>
+      <c r="Z125" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA125" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB125" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC125" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD125" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -11429,6 +13562,23 @@
       <c r="Y126" t="n">
         <v>2</v>
       </c>
+      <c r="Z126" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA126" t="n">
+        <v>40</v>
+      </c>
+      <c r="AB126" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC126" t="n">
+        <v>35</v>
+      </c>
+      <c r="AD126" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -11516,6 +13666,23 @@
       <c r="Y127" t="n">
         <v>-2</v>
       </c>
+      <c r="Z127" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA127" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB127" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC127" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD127" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -11603,6 +13770,23 @@
       <c r="Y128" t="n">
         <v>-5</v>
       </c>
+      <c r="Z128" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA128" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB128" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC128" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD128" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -11690,6 +13874,23 @@
       <c r="Y129" t="n">
         <v>5</v>
       </c>
+      <c r="Z129" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA129" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB129" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC129" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD129" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -11777,6 +13978,23 @@
       <c r="Y130" t="n">
         <v>-10</v>
       </c>
+      <c r="Z130" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA130" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB130" t="n">
+        <v>43</v>
+      </c>
+      <c r="AC130" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD130" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -11864,6 +14082,23 @@
       <c r="Y131" t="n">
         <v>10</v>
       </c>
+      <c r="Z131" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA131" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB131" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC131" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD131" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -11951,6 +14186,23 @@
       <c r="Y132" t="n">
         <v>-26</v>
       </c>
+      <c r="Z132" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA132" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB132" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC132" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD132" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -12038,6 +14290,23 @@
       <c r="Y133" t="n">
         <v>26</v>
       </c>
+      <c r="Z133" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA133" t="n">
+        <v>31</v>
+      </c>
+      <c r="AB133" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC133" t="n">
+        <v>34</v>
+      </c>
+      <c r="AD133" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -12125,6 +14394,23 @@
       <c r="Y134" t="n">
         <v>-3</v>
       </c>
+      <c r="Z134" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA134" t="n">
+        <v>19</v>
+      </c>
+      <c r="AB134" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC134" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD134" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -12212,6 +14498,23 @@
       <c r="Y135" t="n">
         <v>3</v>
       </c>
+      <c r="Z135" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA135" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB135" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC135" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD135" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -12299,6 +14602,23 @@
       <c r="Y136" t="n">
         <v>9</v>
       </c>
+      <c r="Z136" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA136" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB136" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC136" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD136" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -12386,6 +14706,23 @@
       <c r="Y137" t="n">
         <v>-9</v>
       </c>
+      <c r="Z137" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA137" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB137" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC137" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD137" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -12473,6 +14810,23 @@
       <c r="Y138" t="n">
         <v>-11</v>
       </c>
+      <c r="Z138" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA138" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB138" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC138" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD138" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -12560,6 +14914,23 @@
       <c r="Y139" t="n">
         <v>11</v>
       </c>
+      <c r="Z139" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA139" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB139" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC139" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD139" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -12647,6 +15018,23 @@
       <c r="Y140" t="n">
         <v>-3</v>
       </c>
+      <c r="Z140" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA140" t="n">
+        <v>31</v>
+      </c>
+      <c r="AB140" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC140" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD140" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -12734,6 +15122,23 @@
       <c r="Y141" t="n">
         <v>3</v>
       </c>
+      <c r="Z141" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA141" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB141" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC141" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD141" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -12821,6 +15226,23 @@
       <c r="Y142" t="n">
         <v>-9</v>
       </c>
+      <c r="Z142" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA142" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB142" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC142" t="n">
+        <v>34</v>
+      </c>
+      <c r="AD142" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -12908,6 +15330,23 @@
       <c r="Y143" t="n">
         <v>9</v>
       </c>
+      <c r="Z143" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA143" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB143" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC143" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD143" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -12995,6 +15434,23 @@
       <c r="Y144" t="n">
         <v>-26</v>
       </c>
+      <c r="Z144" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA144" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB144" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC144" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD144" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -13082,6 +15538,23 @@
       <c r="Y145" t="n">
         <v>26</v>
       </c>
+      <c r="Z145" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA145" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB145" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC145" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD145" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -13169,6 +15642,23 @@
       <c r="Y146" t="n">
         <v>16</v>
       </c>
+      <c r="Z146" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA146" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB146" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC146" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD146" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -13255,6 +15745,23 @@
       </c>
       <c r="Y147" t="n">
         <v>-16</v>
+      </c>
+      <c r="Z147" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA147" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB147" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC147" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD147" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update GSW stats json & re-create spreadsheets
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD147"/>
+  <dimension ref="A1:AD155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15764,6 +15764,838 @@
         </is>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>56</v>
+      </c>
+      <c r="H148" t="n">
+        <v>97</v>
+      </c>
+      <c r="I148" t="n">
+        <v>0.577</v>
+      </c>
+      <c r="J148" t="n">
+        <v>21</v>
+      </c>
+      <c r="K148" t="n">
+        <v>44</v>
+      </c>
+      <c r="L148" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="M148" t="n">
+        <v>15</v>
+      </c>
+      <c r="N148" t="n">
+        <v>19</v>
+      </c>
+      <c r="O148" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="P148" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q148" t="n">
+        <v>34</v>
+      </c>
+      <c r="R148" t="n">
+        <v>44</v>
+      </c>
+      <c r="S148" t="n">
+        <v>42</v>
+      </c>
+      <c r="T148" t="n">
+        <v>17</v>
+      </c>
+      <c r="U148" t="n">
+        <v>3</v>
+      </c>
+      <c r="V148" t="n">
+        <v>12</v>
+      </c>
+      <c r="W148" t="n">
+        <v>15</v>
+      </c>
+      <c r="X148" t="n">
+        <v>148</v>
+      </c>
+      <c r="Y148" t="n">
+        <v>42</v>
+      </c>
+      <c r="Z148" t="n">
+        <v>44</v>
+      </c>
+      <c r="AA148" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB148" t="n">
+        <v>43</v>
+      </c>
+      <c r="AC148" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD148" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>40</v>
+      </c>
+      <c r="H149" t="n">
+        <v>84</v>
+      </c>
+      <c r="I149" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="J149" t="n">
+        <v>16</v>
+      </c>
+      <c r="K149" t="n">
+        <v>42</v>
+      </c>
+      <c r="L149" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="M149" t="n">
+        <v>10</v>
+      </c>
+      <c r="N149" t="n">
+        <v>16</v>
+      </c>
+      <c r="O149" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="P149" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>27</v>
+      </c>
+      <c r="R149" t="n">
+        <v>34</v>
+      </c>
+      <c r="S149" t="n">
+        <v>30</v>
+      </c>
+      <c r="T149" t="n">
+        <v>4</v>
+      </c>
+      <c r="U149" t="n">
+        <v>3</v>
+      </c>
+      <c r="V149" t="n">
+        <v>21</v>
+      </c>
+      <c r="W149" t="n">
+        <v>20</v>
+      </c>
+      <c r="X149" t="n">
+        <v>106</v>
+      </c>
+      <c r="Y149" t="n">
+        <v>-42</v>
+      </c>
+      <c r="Z149" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA149" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB149" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC149" t="n">
+        <v>33</v>
+      </c>
+      <c r="AD149" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>2025-04-01</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G150" t="n">
+        <v>42</v>
+      </c>
+      <c r="H150" t="n">
+        <v>99</v>
+      </c>
+      <c r="I150" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="J150" t="n">
+        <v>22</v>
+      </c>
+      <c r="K150" t="n">
+        <v>56</v>
+      </c>
+      <c r="L150" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="M150" t="n">
+        <v>28</v>
+      </c>
+      <c r="N150" t="n">
+        <v>28</v>
+      </c>
+      <c r="O150" t="n">
+        <v>1</v>
+      </c>
+      <c r="P150" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>34</v>
+      </c>
+      <c r="R150" t="n">
+        <v>49</v>
+      </c>
+      <c r="S150" t="n">
+        <v>29</v>
+      </c>
+      <c r="T150" t="n">
+        <v>11</v>
+      </c>
+      <c r="U150" t="n">
+        <v>3</v>
+      </c>
+      <c r="V150" t="n">
+        <v>11</v>
+      </c>
+      <c r="W150" t="n">
+        <v>22</v>
+      </c>
+      <c r="X150" t="n">
+        <v>134</v>
+      </c>
+      <c r="Y150" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z150" t="n">
+        <v>45</v>
+      </c>
+      <c r="AA150" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB150" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC150" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD150" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>2025-04-01</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>44</v>
+      </c>
+      <c r="H151" t="n">
+        <v>92</v>
+      </c>
+      <c r="I151" t="n">
+        <v>0.478</v>
+      </c>
+      <c r="J151" t="n">
+        <v>18</v>
+      </c>
+      <c r="K151" t="n">
+        <v>44</v>
+      </c>
+      <c r="L151" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="M151" t="n">
+        <v>19</v>
+      </c>
+      <c r="N151" t="n">
+        <v>22</v>
+      </c>
+      <c r="O151" t="n">
+        <v>0.864</v>
+      </c>
+      <c r="P151" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>35</v>
+      </c>
+      <c r="R151" t="n">
+        <v>43</v>
+      </c>
+      <c r="S151" t="n">
+        <v>22</v>
+      </c>
+      <c r="T151" t="n">
+        <v>7</v>
+      </c>
+      <c r="U151" t="n">
+        <v>6</v>
+      </c>
+      <c r="V151" t="n">
+        <v>16</v>
+      </c>
+      <c r="W151" t="n">
+        <v>23</v>
+      </c>
+      <c r="X151" t="n">
+        <v>125</v>
+      </c>
+      <c r="Y151" t="n">
+        <v>-9</v>
+      </c>
+      <c r="Z151" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA151" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB151" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC151" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD151" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>2025-04-03</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>39</v>
+      </c>
+      <c r="H152" t="n">
+        <v>82</v>
+      </c>
+      <c r="I152" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="J152" t="n">
+        <v>19</v>
+      </c>
+      <c r="K152" t="n">
+        <v>42</v>
+      </c>
+      <c r="L152" t="n">
+        <v>0.452</v>
+      </c>
+      <c r="M152" t="n">
+        <v>26</v>
+      </c>
+      <c r="N152" t="n">
+        <v>31</v>
+      </c>
+      <c r="O152" t="n">
+        <v>0.839</v>
+      </c>
+      <c r="P152" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q152" t="n">
+        <v>32</v>
+      </c>
+      <c r="R152" t="n">
+        <v>46</v>
+      </c>
+      <c r="S152" t="n">
+        <v>30</v>
+      </c>
+      <c r="T152" t="n">
+        <v>5</v>
+      </c>
+      <c r="U152" t="n">
+        <v>2</v>
+      </c>
+      <c r="V152" t="n">
+        <v>13</v>
+      </c>
+      <c r="W152" t="n">
+        <v>21</v>
+      </c>
+      <c r="X152" t="n">
+        <v>123</v>
+      </c>
+      <c r="Y152" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z152" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA152" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB152" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC152" t="n">
+        <v>35</v>
+      </c>
+      <c r="AD152" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>2025-04-03</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>39</v>
+      </c>
+      <c r="H153" t="n">
+        <v>86</v>
+      </c>
+      <c r="I153" t="n">
+        <v>0.453</v>
+      </c>
+      <c r="J153" t="n">
+        <v>18</v>
+      </c>
+      <c r="K153" t="n">
+        <v>47</v>
+      </c>
+      <c r="L153" t="n">
+        <v>0.383</v>
+      </c>
+      <c r="M153" t="n">
+        <v>20</v>
+      </c>
+      <c r="N153" t="n">
+        <v>23</v>
+      </c>
+      <c r="O153" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="P153" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>25</v>
+      </c>
+      <c r="R153" t="n">
+        <v>39</v>
+      </c>
+      <c r="S153" t="n">
+        <v>23</v>
+      </c>
+      <c r="T153" t="n">
+        <v>5</v>
+      </c>
+      <c r="U153" t="n">
+        <v>3</v>
+      </c>
+      <c r="V153" t="n">
+        <v>8</v>
+      </c>
+      <c r="W153" t="n">
+        <v>23</v>
+      </c>
+      <c r="X153" t="n">
+        <v>116</v>
+      </c>
+      <c r="Y153" t="n">
+        <v>-7</v>
+      </c>
+      <c r="Z153" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA153" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB153" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC153" t="n">
+        <v>39</v>
+      </c>
+      <c r="AD153" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>2025-04-04</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G154" t="n">
+        <v>40</v>
+      </c>
+      <c r="H154" t="n">
+        <v>74</v>
+      </c>
+      <c r="I154" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="J154" t="n">
+        <v>12</v>
+      </c>
+      <c r="K154" t="n">
+        <v>31</v>
+      </c>
+      <c r="L154" t="n">
+        <v>0.387</v>
+      </c>
+      <c r="M154" t="n">
+        <v>12</v>
+      </c>
+      <c r="N154" t="n">
+        <v>13</v>
+      </c>
+      <c r="O154" t="n">
+        <v>0.923</v>
+      </c>
+      <c r="P154" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q154" t="n">
+        <v>31</v>
+      </c>
+      <c r="R154" t="n">
+        <v>38</v>
+      </c>
+      <c r="S154" t="n">
+        <v>28</v>
+      </c>
+      <c r="T154" t="n">
+        <v>8</v>
+      </c>
+      <c r="U154" t="n">
+        <v>4</v>
+      </c>
+      <c r="V154" t="n">
+        <v>25</v>
+      </c>
+      <c r="W154" t="n">
+        <v>18</v>
+      </c>
+      <c r="X154" t="n">
+        <v>104</v>
+      </c>
+      <c r="Y154" t="n">
+        <v>-14</v>
+      </c>
+      <c r="Z154" t="n">
+        <v>44</v>
+      </c>
+      <c r="AA154" t="n">
+        <v>16</v>
+      </c>
+      <c r="AB154" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC154" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD154" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>2025-04-04</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G155" t="n">
+        <v>43</v>
+      </c>
+      <c r="H155" t="n">
+        <v>88</v>
+      </c>
+      <c r="I155" t="n">
+        <v>0.489</v>
+      </c>
+      <c r="J155" t="n">
+        <v>16</v>
+      </c>
+      <c r="K155" t="n">
+        <v>38</v>
+      </c>
+      <c r="L155" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="M155" t="n">
+        <v>16</v>
+      </c>
+      <c r="N155" t="n">
+        <v>18</v>
+      </c>
+      <c r="O155" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="P155" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q155" t="n">
+        <v>25</v>
+      </c>
+      <c r="R155" t="n">
+        <v>36</v>
+      </c>
+      <c r="S155" t="n">
+        <v>25</v>
+      </c>
+      <c r="T155" t="n">
+        <v>14</v>
+      </c>
+      <c r="U155" t="n">
+        <v>2</v>
+      </c>
+      <c r="V155" t="n">
+        <v>13</v>
+      </c>
+      <c r="W155" t="n">
+        <v>15</v>
+      </c>
+      <c r="X155" t="n">
+        <v>118</v>
+      </c>
+      <c r="Y155" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z155" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA155" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB155" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC155" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD155" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GSW spreadsheets based on latest box scores
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD155"/>
+  <dimension ref="A1:AD161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16596,6 +16596,630 @@
         </is>
       </c>
     </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>2025-04-06</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G156" t="n">
+        <v>45</v>
+      </c>
+      <c r="H156" t="n">
+        <v>93</v>
+      </c>
+      <c r="I156" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="J156" t="n">
+        <v>10</v>
+      </c>
+      <c r="K156" t="n">
+        <v>30</v>
+      </c>
+      <c r="L156" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="M156" t="n">
+        <v>6</v>
+      </c>
+      <c r="N156" t="n">
+        <v>16</v>
+      </c>
+      <c r="O156" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="P156" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q156" t="n">
+        <v>33</v>
+      </c>
+      <c r="R156" t="n">
+        <v>49</v>
+      </c>
+      <c r="S156" t="n">
+        <v>26</v>
+      </c>
+      <c r="T156" t="n">
+        <v>11</v>
+      </c>
+      <c r="U156" t="n">
+        <v>7</v>
+      </c>
+      <c r="V156" t="n">
+        <v>15</v>
+      </c>
+      <c r="W156" t="n">
+        <v>15</v>
+      </c>
+      <c r="X156" t="n">
+        <v>106</v>
+      </c>
+      <c r="Y156" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z156" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA156" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB156" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC156" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD156" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>2025-04-06</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G157" t="n">
+        <v>37</v>
+      </c>
+      <c r="H157" t="n">
+        <v>89</v>
+      </c>
+      <c r="I157" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="J157" t="n">
+        <v>16</v>
+      </c>
+      <c r="K157" t="n">
+        <v>43</v>
+      </c>
+      <c r="L157" t="n">
+        <v>0.372</v>
+      </c>
+      <c r="M157" t="n">
+        <v>6</v>
+      </c>
+      <c r="N157" t="n">
+        <v>11</v>
+      </c>
+      <c r="O157" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="P157" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q157" t="n">
+        <v>31</v>
+      </c>
+      <c r="R157" t="n">
+        <v>46</v>
+      </c>
+      <c r="S157" t="n">
+        <v>28</v>
+      </c>
+      <c r="T157" t="n">
+        <v>12</v>
+      </c>
+      <c r="U157" t="n">
+        <v>2</v>
+      </c>
+      <c r="V157" t="n">
+        <v>20</v>
+      </c>
+      <c r="W157" t="n">
+        <v>14</v>
+      </c>
+      <c r="X157" t="n">
+        <v>96</v>
+      </c>
+      <c r="Y157" t="n">
+        <v>-10</v>
+      </c>
+      <c r="Z157" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA157" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB157" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC157" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD157" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>PHX</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>45</v>
+      </c>
+      <c r="H158" t="n">
+        <v>93</v>
+      </c>
+      <c r="I158" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="J158" t="n">
+        <v>15</v>
+      </c>
+      <c r="K158" t="n">
+        <v>40</v>
+      </c>
+      <c r="L158" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="M158" t="n">
+        <v>28</v>
+      </c>
+      <c r="N158" t="n">
+        <v>34</v>
+      </c>
+      <c r="O158" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="P158" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>38</v>
+      </c>
+      <c r="R158" t="n">
+        <v>57</v>
+      </c>
+      <c r="S158" t="n">
+        <v>31</v>
+      </c>
+      <c r="T158" t="n">
+        <v>14</v>
+      </c>
+      <c r="U158" t="n">
+        <v>3</v>
+      </c>
+      <c r="V158" t="n">
+        <v>15</v>
+      </c>
+      <c r="W158" t="n">
+        <v>10</v>
+      </c>
+      <c r="X158" t="n">
+        <v>133</v>
+      </c>
+      <c r="Y158" t="n">
+        <v>38</v>
+      </c>
+      <c r="Z158" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA158" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB158" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC158" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD158" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>PHX</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>35</v>
+      </c>
+      <c r="H159" t="n">
+        <v>88</v>
+      </c>
+      <c r="I159" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="J159" t="n">
+        <v>12</v>
+      </c>
+      <c r="K159" t="n">
+        <v>43</v>
+      </c>
+      <c r="L159" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="M159" t="n">
+        <v>13</v>
+      </c>
+      <c r="N159" t="n">
+        <v>15</v>
+      </c>
+      <c r="O159" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="P159" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>28</v>
+      </c>
+      <c r="R159" t="n">
+        <v>41</v>
+      </c>
+      <c r="S159" t="n">
+        <v>22</v>
+      </c>
+      <c r="T159" t="n">
+        <v>12</v>
+      </c>
+      <c r="U159" t="n">
+        <v>4</v>
+      </c>
+      <c r="V159" t="n">
+        <v>19</v>
+      </c>
+      <c r="W159" t="n">
+        <v>19</v>
+      </c>
+      <c r="X159" t="n">
+        <v>95</v>
+      </c>
+      <c r="Y159" t="n">
+        <v>-38</v>
+      </c>
+      <c r="Z159" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA159" t="n">
+        <v>19</v>
+      </c>
+      <c r="AB159" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC159" t="n">
+        <v>34</v>
+      </c>
+      <c r="AD159" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>39</v>
+      </c>
+      <c r="H160" t="n">
+        <v>81</v>
+      </c>
+      <c r="I160" t="n">
+        <v>0.481</v>
+      </c>
+      <c r="J160" t="n">
+        <v>18</v>
+      </c>
+      <c r="K160" t="n">
+        <v>46</v>
+      </c>
+      <c r="L160" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="M160" t="n">
+        <v>18</v>
+      </c>
+      <c r="N160" t="n">
+        <v>21</v>
+      </c>
+      <c r="O160" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="P160" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q160" t="n">
+        <v>33</v>
+      </c>
+      <c r="R160" t="n">
+        <v>43</v>
+      </c>
+      <c r="S160" t="n">
+        <v>23</v>
+      </c>
+      <c r="T160" t="n">
+        <v>6</v>
+      </c>
+      <c r="U160" t="n">
+        <v>5</v>
+      </c>
+      <c r="V160" t="n">
+        <v>13</v>
+      </c>
+      <c r="W160" t="n">
+        <v>23</v>
+      </c>
+      <c r="X160" t="n">
+        <v>114</v>
+      </c>
+      <c r="Y160" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z160" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA160" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB160" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC160" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD160" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G161" t="n">
+        <v>36</v>
+      </c>
+      <c r="H161" t="n">
+        <v>86</v>
+      </c>
+      <c r="I161" t="n">
+        <v>0.419</v>
+      </c>
+      <c r="J161" t="n">
+        <v>16</v>
+      </c>
+      <c r="K161" t="n">
+        <v>48</v>
+      </c>
+      <c r="L161" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="M161" t="n">
+        <v>23</v>
+      </c>
+      <c r="N161" t="n">
+        <v>28</v>
+      </c>
+      <c r="O161" t="n">
+        <v>0.821</v>
+      </c>
+      <c r="P161" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q161" t="n">
+        <v>29</v>
+      </c>
+      <c r="R161" t="n">
+        <v>45</v>
+      </c>
+      <c r="S161" t="n">
+        <v>29</v>
+      </c>
+      <c r="T161" t="n">
+        <v>8</v>
+      </c>
+      <c r="U161" t="n">
+        <v>2</v>
+      </c>
+      <c r="V161" t="n">
+        <v>10</v>
+      </c>
+      <c r="W161" t="n">
+        <v>19</v>
+      </c>
+      <c r="X161" t="n">
+        <v>111</v>
+      </c>
+      <c r="Y161" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Z161" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA161" t="n">
+        <v>19</v>
+      </c>
+      <c r="AB161" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC161" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD161" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GSW speadsheets with final games of regular season
</commit_message>
<xml_diff>
--- a/data/gsw_box_score_team_stats.xlsx
+++ b/data/gsw_box_score_team_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD161"/>
+  <dimension ref="A1:AD165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17220,6 +17220,422 @@
         </is>
       </c>
     </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>33</v>
+      </c>
+      <c r="H162" t="n">
+        <v>83</v>
+      </c>
+      <c r="I162" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="J162" t="n">
+        <v>14</v>
+      </c>
+      <c r="K162" t="n">
+        <v>44</v>
+      </c>
+      <c r="L162" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="M162" t="n">
+        <v>23</v>
+      </c>
+      <c r="N162" t="n">
+        <v>28</v>
+      </c>
+      <c r="O162" t="n">
+        <v>0.821</v>
+      </c>
+      <c r="P162" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q162" t="n">
+        <v>38</v>
+      </c>
+      <c r="R162" t="n">
+        <v>45</v>
+      </c>
+      <c r="S162" t="n">
+        <v>26</v>
+      </c>
+      <c r="T162" t="n">
+        <v>15</v>
+      </c>
+      <c r="U162" t="n">
+        <v>7</v>
+      </c>
+      <c r="V162" t="n">
+        <v>14</v>
+      </c>
+      <c r="W162" t="n">
+        <v>19</v>
+      </c>
+      <c r="X162" t="n">
+        <v>103</v>
+      </c>
+      <c r="Y162" t="n">
+        <v>17</v>
+      </c>
+      <c r="Z162" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA162" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB162" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC162" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD162" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>240:00</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>32</v>
+      </c>
+      <c r="H163" t="n">
+        <v>85</v>
+      </c>
+      <c r="I163" t="n">
+        <v>0.376</v>
+      </c>
+      <c r="J163" t="n">
+        <v>6</v>
+      </c>
+      <c r="K163" t="n">
+        <v>30</v>
+      </c>
+      <c r="L163" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M163" t="n">
+        <v>16</v>
+      </c>
+      <c r="N163" t="n">
+        <v>22</v>
+      </c>
+      <c r="O163" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="P163" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q163" t="n">
+        <v>39</v>
+      </c>
+      <c r="R163" t="n">
+        <v>52</v>
+      </c>
+      <c r="S163" t="n">
+        <v>21</v>
+      </c>
+      <c r="T163" t="n">
+        <v>9</v>
+      </c>
+      <c r="U163" t="n">
+        <v>5</v>
+      </c>
+      <c r="V163" t="n">
+        <v>22</v>
+      </c>
+      <c r="W163" t="n">
+        <v>20</v>
+      </c>
+      <c r="X163" t="n">
+        <v>86</v>
+      </c>
+      <c r="Y163" t="n">
+        <v>-17</v>
+      </c>
+      <c r="Z163" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA163" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB163" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC163" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD163" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>away</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>265:00</t>
+        </is>
+      </c>
+      <c r="G164" t="n">
+        <v>48</v>
+      </c>
+      <c r="H164" t="n">
+        <v>86</v>
+      </c>
+      <c r="I164" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="J164" t="n">
+        <v>14</v>
+      </c>
+      <c r="K164" t="n">
+        <v>30</v>
+      </c>
+      <c r="L164" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="M164" t="n">
+        <v>14</v>
+      </c>
+      <c r="N164" t="n">
+        <v>18</v>
+      </c>
+      <c r="O164" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="P164" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q164" t="n">
+        <v>33</v>
+      </c>
+      <c r="R164" t="n">
+        <v>42</v>
+      </c>
+      <c r="S164" t="n">
+        <v>28</v>
+      </c>
+      <c r="T164" t="n">
+        <v>11</v>
+      </c>
+      <c r="U164" t="n">
+        <v>3</v>
+      </c>
+      <c r="V164" t="n">
+        <v>16</v>
+      </c>
+      <c r="W164" t="n">
+        <v>21</v>
+      </c>
+      <c r="X164" t="n">
+        <v>124</v>
+      </c>
+      <c r="Y164" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z164" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA164" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB164" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC164" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD164" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>265:00</t>
+        </is>
+      </c>
+      <c r="G165" t="n">
+        <v>43</v>
+      </c>
+      <c r="H165" t="n">
+        <v>79</v>
+      </c>
+      <c r="I165" t="n">
+        <v>0.544</v>
+      </c>
+      <c r="J165" t="n">
+        <v>15</v>
+      </c>
+      <c r="K165" t="n">
+        <v>33</v>
+      </c>
+      <c r="L165" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="M165" t="n">
+        <v>18</v>
+      </c>
+      <c r="N165" t="n">
+        <v>23</v>
+      </c>
+      <c r="O165" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="P165" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q165" t="n">
+        <v>22</v>
+      </c>
+      <c r="R165" t="n">
+        <v>25</v>
+      </c>
+      <c r="S165" t="n">
+        <v>31</v>
+      </c>
+      <c r="T165" t="n">
+        <v>11</v>
+      </c>
+      <c r="U165" t="n">
+        <v>6</v>
+      </c>
+      <c r="V165" t="n">
+        <v>15</v>
+      </c>
+      <c r="W165" t="n">
+        <v>20</v>
+      </c>
+      <c r="X165" t="n">
+        <v>119</v>
+      </c>
+      <c r="Y165" t="n">
+        <v>-5</v>
+      </c>
+      <c r="Z165" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA165" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB165" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC165" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD165" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>